<commit_message>
Enhanced py files and add new col to files tab
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C010308-24F3-BD40-AD7C-213900FD6BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EC742E-F3C3-E843-902C-D988D6BB0FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39980" yWindow="3520" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -74,13 +74,17 @@
     FROM 
         df_participant sp
     JOIN 
-        df_study s
-    ON 
-        sp."study.phs_accession" = s.phs_accession
+        df_study s ON sp."study.phs_accession" = s.phs_accession
     JOIN 
-        df_sample smp
-    ON 
-        smp."participant.study_participant_id" = sp.study_participant_id
+        df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+    JOIN
+        df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+    JOIN
+        df_program p ON p.program_acronym = s."program.program_acronym"
+    JOIN
+        df_file f1 ON f1."sample.sample_id" = smp.sample_id
+    JOIN
+        df_genomic_info gi ON gi."file.file_id" = f1.file_id
     WHERE 
         s.phs_accession = 'phs001287' AND sp.gender = 'Female'
 ),
@@ -121,33 +125,6 @@
   </si>
   <si>
     <t>SELECT
-    COUNT(DISTINCT s.study_name) AS "Studies",
-    COUNT(DISTINCT sp.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT f.file_id) AS "Files"
-FROM 
-    df_participant sp
-JOIN 
-    df_study s
-ON 
-    sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp
-ON 
-    smp."participant.study_participant_id" = sp.study_participant_id
-JOIN 
-    df_program p
-ON
-    p.program_acronym = s."program.program_acronym"
-JOIN
-    df_file f
-ON
-    f."sample.sample_id" = smp.sample_id
-WHERE 
-    s.phs_accession='phs001287' AND sp.gender = 'Female'</t>
-  </si>
-  <si>
-    <t>SELECT
     DISTINCT (smp.sample_id) AS "Sample ID",
     sp.participant_id AS "Participant ID", 
     s.study_name AS "Study Name",
@@ -157,17 +134,21 @@
 FROM 
     df_participant sp
 JOIN 
-    df_study s
-ON 
-    sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp
-ON 
-    smp."participant.study_participant_id" = sp.study_participant_id
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
 WHERE 
     s.phs_accession = 'phs001287' AND sp.gender = 'Female'
 ORDER BY 
-    smp.sample_id  ASC
+    smp.sample_id ASC
 LIMIT 100;</t>
   </si>
   <si>
@@ -188,7 +169,8 @@
             WHERE smp."participant.study_participant_id" = sp.study_participant_id
         ) smp
     ), '') AS "Sample Id",
-    f1.file_type AS "File Type"
+    f1.file_type AS "File Type",
+    gi.library_strategy AS "Library Strategy"
 FROM 
     df_study s
 INNER JOIN 
@@ -197,6 +179,12 @@
     df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
 INNER JOIN 
     df_file f1 ON f1."sample.sample_id" = smp.sample_id
+INNER JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+INNER JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
 WHERE 
     s.phs_accession = 'phs001287' AND sp.gender = 'Female'
 GROUP BY
@@ -204,26 +192,43 @@
     s.study_name,
     s.phs_accession,
     sp.participant_id,
-    f1.file_type
+    f1.file_type,
+    gi.library_strategy
 ORDER BY 
     f1.file_name ASC
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT s.study_name) AS "Studies",
+    COUNT(DISTINCT sp.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    COUNT(DISTINCT f.file_id) AS "Files"
+FROM 
+    df_participant sp
+JOIN 
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN 
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN 
+    df_file f ON f."sample.sample_id" = smp.sample_id
+JOIN 
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN 
+    df_genomic_info gi ON gi."file.file_id" = f.file_id
+WHERE 
+    s.phs_accession = 'phs001287' AND sp.gender = 'Female';</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -276,17 +281,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -609,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,8 +647,8 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -655,12 +657,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="372" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -669,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -681,7 +683,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed CDS QuickRun suite and Related tests
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0597CA33-6172-9A4C-8938-BB52B6E9103E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4E006-2BE6-8047-97DA-3E8B40B8C414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39980" yWindow="3520" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -198,9 +198,7 @@
     DISTINCT (smp.sample_id) AS "Sample ID",
     sp.participant_id AS "Participant ID", 
     s.study_name AS "Study Name",
-    s.phs_accession AS Accession,
-    smp.sample_tumor_status AS "Sample Tumor Status",
-    smp.sample_type AS "Sample Type"
+    s.phs_accession AS Accession
 FROM 
     df_participant sp
 JOIN 
@@ -667,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="404" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
1437 and 1287 working versions
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs001287_Gender_Female.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/CDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4E006-2BE6-8047-97DA-3E8B40B8C414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E68302-4430-B34A-8E76-F31ED3752107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39980" yWindow="3520" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-4140" yWindow="-22080" windowWidth="35040" windowHeight="22500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,6 +125,32 @@
   </si>
   <si>
     <t>SELECT
+    DISTINCT (smp.sample_id) AS "Sample ID",
+    sp.participant_id AS "Participant ID", 
+    s.study_name AS "Study Name",
+    s.phs_accession AS Accession
+FROM 
+    df_participant sp
+JOIN 
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+WHERE 
+    s.phs_accession = 'phs001287' AND sp.gender = 'Female'
+ORDER BY 
+    smp.sample_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
     f1.file_name AS "File Name",
     s.study_name AS "Study Name",
     s.phs_accession AS "Accession",
@@ -142,7 +168,8 @@
         ) smp
     ), '') AS "Sample Id",
     f1.file_type AS "File Type",
-    gi.library_strategy AS "Library Strategy"
+    gi.library_strategy AS "Library Strategy",
+    '' AS "Supplementary Files"
 FROM 
     df_study s
 INNER JOIN 
@@ -193,40 +220,28 @@
 WHERE 
     s.phs_accession = 'phs001287' AND sp.gender = 'Female';</t>
   </si>
-  <si>
-    <t>SELECT
-    DISTINCT (smp.sample_id) AS "Sample ID",
-    sp.participant_id AS "Participant ID", 
-    s.study_name AS "Study Name",
-    s.phs_accession AS Accession
-FROM 
-    df_participant sp
-JOIN 
-    df_study s ON sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-JOIN
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-WHERE 
-    s.phs_accession = 'phs001287' AND sp.gender = 'Female'
-ORDER BY 
-    smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -286,14 +301,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -655,8 +676,8 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -670,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -678,8 +699,8 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -691,7 +712,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>